<commit_message>
made the func around proper nouns better (still need to test tho)
</commit_message>
<xml_diff>
--- a/files/Pemtara_Eng_Dictionary.xlsx
+++ b/files/Pemtara_Eng_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voidant/Desktop/calculations/Pemtara-Dictionary/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F9068D-5394-9644-BB18-EA203E99E48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4376D-512C-BB47-AEA6-D39182D3EFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16360" yWindow="500" windowWidth="17240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5629" uniqueCount="3909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5679" uniqueCount="3910">
   <si>
     <t>Pemtara</t>
   </si>
@@ -11759,6 +11759,9 @@
   </si>
   <si>
     <t>Fenesuera</t>
+  </si>
+  <si>
+    <t>proper</t>
   </si>
 </sst>
 </file>
@@ -12281,14 +12284,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -12672,8 +12674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L902"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12767,6 +12769,9 @@
       <c r="A4" t="s">
         <v>3866</v>
       </c>
+      <c r="B4" t="s">
+        <v>3909</v>
+      </c>
       <c r="H4" t="s">
         <v>3861</v>
       </c>
@@ -13075,6 +13080,9 @@
       <c r="A20" t="s">
         <v>3764</v>
       </c>
+      <c r="B20" t="s">
+        <v>3909</v>
+      </c>
       <c r="H20" t="s">
         <v>3790</v>
       </c>
@@ -13169,6 +13177,9 @@
       <c r="A25" t="s">
         <v>3888</v>
       </c>
+      <c r="B25" t="s">
+        <v>3909</v>
+      </c>
       <c r="H25" t="s">
         <v>3887</v>
       </c>
@@ -13415,6 +13426,9 @@
       <c r="A36" t="s">
         <v>3848</v>
       </c>
+      <c r="B36" t="s">
+        <v>3909</v>
+      </c>
       <c r="H36" t="s">
         <v>3850</v>
       </c>
@@ -14070,6 +14084,9 @@
       <c r="A66" t="s">
         <v>3876</v>
       </c>
+      <c r="B66" t="s">
+        <v>3909</v>
+      </c>
       <c r="H66" t="s">
         <v>3849</v>
       </c>
@@ -14079,7 +14096,7 @@
       <c r="K66" t="s">
         <v>3851</v>
       </c>
-      <c r="L66" s="8" t="s">
+      <c r="L66" s="7" t="s">
         <v>3852</v>
       </c>
     </row>
@@ -14110,6 +14127,9 @@
       <c r="A68" t="s">
         <v>3844</v>
       </c>
+      <c r="B68" t="s">
+        <v>3909</v>
+      </c>
       <c r="H68" t="s">
         <v>3845</v>
       </c>
@@ -14192,6 +14212,9 @@
       <c r="A72" t="s">
         <v>3875</v>
       </c>
+      <c r="B72" t="s">
+        <v>3909</v>
+      </c>
       <c r="H72" t="s">
         <v>3855</v>
       </c>
@@ -14201,7 +14224,7 @@
       <c r="K72" t="s">
         <v>3853</v>
       </c>
-      <c r="L72" s="8" t="s">
+      <c r="L72" s="7" t="s">
         <v>3854</v>
       </c>
     </row>
@@ -14290,6 +14313,9 @@
       <c r="A77" t="s">
         <v>3901</v>
       </c>
+      <c r="B77" t="s">
+        <v>3909</v>
+      </c>
       <c r="H77" t="s">
         <v>3862</v>
       </c>
@@ -14727,6 +14753,9 @@
       <c r="A97" t="s">
         <v>3908</v>
       </c>
+      <c r="B97" t="s">
+        <v>3909</v>
+      </c>
       <c r="H97" t="s">
         <v>3907</v>
       </c>
@@ -15356,6 +15385,9 @@
       <c r="A125" t="s">
         <v>3821</v>
       </c>
+      <c r="B125" t="s">
+        <v>3909</v>
+      </c>
       <c r="H125" t="s">
         <v>3740</v>
       </c>
@@ -15545,6 +15577,9 @@
       <c r="A134" t="s">
         <v>315</v>
       </c>
+      <c r="B134" t="s">
+        <v>3909</v>
+      </c>
       <c r="D134" t="s">
         <v>316</v>
       </c>
@@ -15721,6 +15756,9 @@
       <c r="A144" t="s">
         <v>3835</v>
       </c>
+      <c r="B144" t="s">
+        <v>3909</v>
+      </c>
       <c r="H144" t="s">
         <v>3834</v>
       </c>
@@ -16979,6 +17017,9 @@
       <c r="A206" t="s">
         <v>3766</v>
       </c>
+      <c r="B206" t="s">
+        <v>3909</v>
+      </c>
       <c r="H206" t="s">
         <v>3793</v>
       </c>
@@ -17114,6 +17155,9 @@
       <c r="A214" t="s">
         <v>3826</v>
       </c>
+      <c r="B214" t="s">
+        <v>3909</v>
+      </c>
       <c r="H214" t="s">
         <v>3741</v>
       </c>
@@ -17128,6 +17172,9 @@
       <c r="A215" t="s">
         <v>3783</v>
       </c>
+      <c r="B215" t="s">
+        <v>3909</v>
+      </c>
       <c r="H215" t="s">
         <v>3800</v>
       </c>
@@ -17737,6 +17784,9 @@
       <c r="A244" t="s">
         <v>506</v>
       </c>
+      <c r="B244" t="s">
+        <v>3909</v>
+      </c>
       <c r="D244" t="s">
         <v>507</v>
       </c>
@@ -18215,6 +18265,9 @@
       <c r="A264" t="s">
         <v>3757</v>
       </c>
+      <c r="B264" t="s">
+        <v>3909</v>
+      </c>
       <c r="H264" t="s">
         <v>3791</v>
       </c>
@@ -18692,6 +18745,9 @@
       <c r="A285" t="s">
         <v>3896</v>
       </c>
+      <c r="B285" t="s">
+        <v>3909</v>
+      </c>
       <c r="H285" t="s">
         <v>3895</v>
       </c>
@@ -19204,6 +19260,9 @@
       <c r="A308" t="s">
         <v>3870</v>
       </c>
+      <c r="B308" t="s">
+        <v>3909</v>
+      </c>
       <c r="H308" t="s">
         <v>3872</v>
       </c>
@@ -19218,6 +19277,9 @@
       <c r="A309" t="s">
         <v>3743</v>
       </c>
+      <c r="B309" t="s">
+        <v>3909</v>
+      </c>
       <c r="H309" t="s">
         <v>3840</v>
       </c>
@@ -19782,13 +19844,16 @@
       <c r="A337" t="s">
         <v>3808</v>
       </c>
+      <c r="B337" t="s">
+        <v>3909</v>
+      </c>
       <c r="H337" t="s">
         <v>3806</v>
       </c>
       <c r="J337" t="s">
         <v>17</v>
       </c>
-      <c r="K337" s="7" t="s">
+      <c r="K337" s="6" t="s">
         <v>3807</v>
       </c>
     </row>
@@ -19928,6 +19993,9 @@
       <c r="A344" t="s">
         <v>3842</v>
       </c>
+      <c r="B344" t="s">
+        <v>3909</v>
+      </c>
       <c r="H344" t="s">
         <v>3841</v>
       </c>
@@ -20401,6 +20469,9 @@
       <c r="A366" t="s">
         <v>3902</v>
       </c>
+      <c r="B366" t="s">
+        <v>3909</v>
+      </c>
       <c r="H366" t="s">
         <v>3873</v>
       </c>
@@ -20528,7 +20599,7 @@
         <v>824</v>
       </c>
       <c r="B372" t="s">
-        <v>2502</v>
+        <v>3909</v>
       </c>
       <c r="H372" t="s">
         <v>825</v>
@@ -21186,6 +21257,9 @@
       <c r="A405" t="s">
         <v>3779</v>
       </c>
+      <c r="B405" t="s">
+        <v>3909</v>
+      </c>
       <c r="H405" t="s">
         <v>3799</v>
       </c>
@@ -21256,6 +21330,9 @@
       <c r="A408" t="s">
         <v>3889</v>
       </c>
+      <c r="B408" t="s">
+        <v>3909</v>
+      </c>
       <c r="H408" t="s">
         <v>3891</v>
       </c>
@@ -21271,7 +21348,7 @@
         <v>890</v>
       </c>
       <c r="B409" t="s">
-        <v>2502</v>
+        <v>3909</v>
       </c>
       <c r="H409" t="s">
         <v>891</v>
@@ -21654,6 +21731,9 @@
       <c r="A426" t="s">
         <v>3789</v>
       </c>
+      <c r="B426" t="s">
+        <v>3909</v>
+      </c>
       <c r="H426" t="s">
         <v>3802</v>
       </c>
@@ -21725,6 +21805,9 @@
       <c r="A430" t="s">
         <v>3833</v>
       </c>
+      <c r="B430" t="s">
+        <v>3909</v>
+      </c>
       <c r="H430" t="s">
         <v>3839</v>
       </c>
@@ -21888,6 +21971,9 @@
       <c r="A438" t="s">
         <v>3894</v>
       </c>
+      <c r="B438" t="s">
+        <v>3909</v>
+      </c>
       <c r="H438" t="s">
         <v>3892</v>
       </c>
@@ -22039,6 +22125,9 @@
       <c r="A446" t="s">
         <v>3818</v>
       </c>
+      <c r="B446" t="s">
+        <v>3909</v>
+      </c>
       <c r="H446" t="s">
         <v>3738</v>
       </c>
@@ -22099,6 +22188,9 @@
       <c r="A449" t="s">
         <v>3828</v>
       </c>
+      <c r="B449" t="s">
+        <v>3909</v>
+      </c>
       <c r="H449" t="s">
         <v>3838</v>
       </c>
@@ -22544,6 +22636,9 @@
       <c r="A472" t="s">
         <v>3774</v>
       </c>
+      <c r="B472" t="s">
+        <v>3909</v>
+      </c>
       <c r="H472" t="s">
         <v>3796</v>
       </c>
@@ -22725,6 +22820,9 @@
       <c r="A481" t="s">
         <v>3755</v>
       </c>
+      <c r="B481" t="s">
+        <v>3909</v>
+      </c>
       <c r="H481" t="s">
         <v>3735</v>
       </c>
@@ -22799,6 +22897,9 @@
       <c r="A485" t="s">
         <v>3906</v>
       </c>
+      <c r="B485" t="s">
+        <v>3909</v>
+      </c>
       <c r="H485" t="s">
         <v>3899</v>
       </c>
@@ -23387,6 +23488,9 @@
       <c r="A514" t="s">
         <v>3883</v>
       </c>
+      <c r="B514" t="s">
+        <v>3909</v>
+      </c>
       <c r="H514" t="s">
         <v>3884</v>
       </c>
@@ -23596,13 +23700,16 @@
       <c r="A523" t="s">
         <v>3733</v>
       </c>
+      <c r="B523" t="s">
+        <v>3909</v>
+      </c>
       <c r="H523" t="s">
         <v>3794</v>
       </c>
       <c r="J523" t="s">
         <v>105</v>
       </c>
-      <c r="K523" s="6" t="s">
+      <c r="K523" t="s">
         <v>3768</v>
       </c>
       <c r="L523" s="1" t="s">
@@ -23653,6 +23760,9 @@
       <c r="A526" t="s">
         <v>3773</v>
       </c>
+      <c r="B526" t="s">
+        <v>3909</v>
+      </c>
       <c r="H526" t="s">
         <v>3797</v>
       </c>
@@ -23733,6 +23843,9 @@
       <c r="A530" t="s">
         <v>3762</v>
       </c>
+      <c r="B530" t="s">
+        <v>3909</v>
+      </c>
       <c r="H530" t="s">
         <v>3792</v>
       </c>
@@ -24290,6 +24403,9 @@
       <c r="A556" t="s">
         <v>3749</v>
       </c>
+      <c r="B556" t="s">
+        <v>3909</v>
+      </c>
       <c r="H556" t="s">
         <v>3885</v>
       </c>
@@ -24708,6 +24824,9 @@
       <c r="A577" t="s">
         <v>3784</v>
       </c>
+      <c r="B577" t="s">
+        <v>3909</v>
+      </c>
       <c r="H577" t="s">
         <v>3801</v>
       </c>
@@ -24877,13 +24996,16 @@
       <c r="A586" t="s">
         <v>3869</v>
       </c>
+      <c r="B586" t="s">
+        <v>3909</v>
+      </c>
       <c r="H586" t="s">
         <v>3871</v>
       </c>
       <c r="J586" t="s">
         <v>3868</v>
       </c>
-      <c r="K586" s="7" t="s">
+      <c r="K586" s="6" t="s">
         <v>3867</v>
       </c>
     </row>
@@ -25081,6 +25203,9 @@
       <c r="A595" t="s">
         <v>3767</v>
       </c>
+      <c r="B595" t="s">
+        <v>3909</v>
+      </c>
       <c r="H595" t="s">
         <v>3795</v>
       </c>
@@ -26188,6 +26313,9 @@
       <c r="A646" t="s">
         <v>3777</v>
       </c>
+      <c r="B646" t="s">
+        <v>3909</v>
+      </c>
       <c r="H646" t="s">
         <v>3798</v>
       </c>
@@ -26503,7 +26631,7 @@
         <v>1385</v>
       </c>
       <c r="B661" t="s">
-        <v>2502</v>
+        <v>3909</v>
       </c>
       <c r="H661" t="s">
         <v>1386</v>
@@ -26856,6 +26984,9 @@
       <c r="A678" t="s">
         <v>3903</v>
       </c>
+      <c r="B678" t="s">
+        <v>3909</v>
+      </c>
       <c r="H678" t="s">
         <v>3880</v>
       </c>
@@ -28314,7 +28445,7 @@
         <v>1532</v>
       </c>
       <c r="B745" t="s">
-        <v>2502</v>
+        <v>3909</v>
       </c>
       <c r="H745" t="s">
         <v>1533</v>
@@ -28848,6 +28979,9 @@
       <c r="A770" t="s">
         <v>3825</v>
       </c>
+      <c r="B770" t="s">
+        <v>3909</v>
+      </c>
       <c r="H770" t="s">
         <v>3824</v>
       </c>
@@ -29934,6 +30068,9 @@
       <c r="A824" t="s">
         <v>3814</v>
       </c>
+      <c r="B824" t="s">
+        <v>3909</v>
+      </c>
       <c r="H824" t="s">
         <v>3737</v>
       </c>
@@ -30514,6 +30651,9 @@
       <c r="A851" t="s">
         <v>3810</v>
       </c>
+      <c r="B851" t="s">
+        <v>3909</v>
+      </c>
       <c r="H851" t="s">
         <v>3811</v>
       </c>
@@ -30529,7 +30669,7 @@
         <v>1728</v>
       </c>
       <c r="B852" t="s">
-        <v>2502</v>
+        <v>3909</v>
       </c>
       <c r="H852" t="s">
         <v>1729</v>
@@ -30655,6 +30795,9 @@
       <c r="A858" t="s">
         <v>3858</v>
       </c>
+      <c r="B858" t="s">
+        <v>3909</v>
+      </c>
       <c r="H858" t="s">
         <v>3747</v>
       </c>
@@ -31168,6 +31311,9 @@
       <c r="A883" t="s">
         <v>3753</v>
       </c>
+      <c r="B883" t="s">
+        <v>3909</v>
+      </c>
       <c r="H883" t="s">
         <v>3897</v>
       </c>
@@ -31385,6 +31531,9 @@
       <c r="A894" t="s">
         <v>3819</v>
       </c>
+      <c r="B894" t="s">
+        <v>3909</v>
+      </c>
       <c r="H894" t="s">
         <v>3739</v>
       </c>
@@ -31458,6 +31607,9 @@
     <row r="898" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A898" t="s">
         <v>3847</v>
+      </c>
+      <c r="B898" t="s">
+        <v>3909</v>
       </c>
       <c r="H898" t="s">
         <v>3846</v>

</xml_diff>